<commit_message>
Construçao dos grafos e inicio das analises
</commit_message>
<xml_diff>
--- a/pl_215.xlsx
+++ b/pl_215.xlsx
@@ -2276,13 +2276,13 @@
     <t>---</t>
   </si>
   <si>
+    <t>id_parlamentar</t>
+  </si>
+  <si>
+    <t>Sigla</t>
+  </si>
+  <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>id_parlamentar</t>
-  </si>
-  <si>
-    <t>Sigla</t>
   </si>
   <si>
     <t>y</t>
@@ -2352,7 +2352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2371,7 +2371,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2675,8 +2674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,19 +2685,19 @@
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s">
         <v>246</v>
       </c>
       <c r="C1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>268</v>
@@ -2706,16 +2705,16 @@
       <c r="E1" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>247</v>
@@ -2730,15 +2729,15 @@
         <v>77</v>
       </c>
       <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>248</v>
@@ -2753,15 +2752,15 @@
         <v>77</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>46</v>
@@ -2776,15 +2775,15 @@
         <v>78</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>47</v>
@@ -2799,15 +2798,15 @@
         <v>82</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>48</v>
@@ -2822,15 +2821,15 @@
         <v>86</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>49</v>
@@ -2845,15 +2844,15 @@
         <v>90</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>50</v>
@@ -2868,15 +2867,15 @@
         <v>94</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="G8" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>249</v>
@@ -2891,15 +2890,15 @@
         <v>98</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="G9" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>250</v>
@@ -2914,15 +2913,15 @@
         <v>102</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G10" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>51</v>
@@ -2937,15 +2936,15 @@
         <v>106</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>52</v>
@@ -2960,15 +2959,15 @@
         <v>110</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="G12" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>53</v>
@@ -2983,15 +2982,15 @@
         <v>114</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="G13" s="5">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>252</v>
@@ -3006,15 +3005,15 @@
         <v>118</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G14" s="5">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>54</v>
@@ -3029,15 +3028,15 @@
         <v>122</v>
       </c>
       <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="G15" s="5">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>251</v>
@@ -3052,15 +3051,15 @@
         <v>126</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="G16" s="5">
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>253</v>
@@ -3075,15 +3074,15 @@
         <v>269</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G17" s="5">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>55</v>
@@ -3098,15 +3097,15 @@
         <v>269</v>
       </c>
       <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="G18" s="5">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>56</v>
@@ -3121,15 +3120,15 @@
         <v>269</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="G19" s="5">
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>254</v>
@@ -3144,15 +3143,15 @@
         <v>269</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="G20" s="5">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>240</v>
@@ -3167,15 +3166,15 @@
         <v>139</v>
       </c>
       <c r="F21" s="4">
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G21" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>57</v>
@@ -3190,15 +3189,15 @@
         <v>269</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="G22" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>255</v>
@@ -3213,15 +3212,15 @@
         <v>269</v>
       </c>
       <c r="F23" s="4">
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="G23" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>58</v>
@@ -3236,15 +3235,15 @@
         <v>269</v>
       </c>
       <c r="F24" s="4">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="G24" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>256</v>
@@ -3259,15 +3258,15 @@
         <v>269</v>
       </c>
       <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="G25" s="5">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>59</v>
@@ -3282,15 +3281,15 @@
         <v>154</v>
       </c>
       <c r="F26" s="4">
-        <v>0</v>
-      </c>
-      <c r="G26" s="4">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="G26" s="5">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>60</v>
@@ -3305,15 +3304,15 @@
         <v>158</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
-      </c>
-      <c r="G27" s="4">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="G27" s="5">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>257</v>
@@ -3328,15 +3327,15 @@
         <v>161</v>
       </c>
       <c r="F28" s="4">
-        <v>0</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="G28" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>61</v>
@@ -3351,15 +3350,15 @@
         <v>164</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="G29" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>62</v>
@@ -3374,15 +3373,15 @@
         <v>168</v>
       </c>
       <c r="F30" s="4">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G30" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>63</v>
@@ -3397,15 +3396,15 @@
         <v>172</v>
       </c>
       <c r="F31" s="4">
-        <v>0</v>
-      </c>
-      <c r="G31" s="4">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G31" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>64</v>
@@ -3420,15 +3419,15 @@
         <v>176</v>
       </c>
       <c r="F32" s="4">
-        <v>0</v>
-      </c>
-      <c r="G32" s="4">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="G32" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>258</v>
@@ -3443,15 +3442,15 @@
         <v>180</v>
       </c>
       <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="G33" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>259</v>
@@ -3466,15 +3465,15 @@
         <v>77</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="G34" s="5">
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>65</v>
@@ -3489,15 +3488,15 @@
         <v>187</v>
       </c>
       <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="4">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="G35" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>66</v>
@@ -3512,15 +3511,15 @@
         <v>191</v>
       </c>
       <c r="F36" s="4">
-        <v>0</v>
-      </c>
-      <c r="G36" s="4">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="G36" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>67</v>
@@ -3535,15 +3534,15 @@
         <v>195</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
-      </c>
-      <c r="G37" s="4">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="G37" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>260</v>
@@ -3558,15 +3557,15 @@
         <v>199</v>
       </c>
       <c r="F38" s="4">
-        <v>0</v>
-      </c>
-      <c r="G38" s="4">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="G38" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>261</v>
@@ -3581,15 +3580,15 @@
         <v>203</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
-      </c>
-      <c r="G39" s="4">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="G39" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>68</v>
@@ -3604,15 +3603,15 @@
         <v>207</v>
       </c>
       <c r="F40" s="4">
-        <v>0</v>
-      </c>
-      <c r="G40" s="4">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="G40" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>69</v>
@@ -3627,15 +3626,15 @@
         <v>209</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
-      </c>
-      <c r="G41" s="4">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="G41" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>70</v>
@@ -3650,15 +3649,15 @@
         <v>212</v>
       </c>
       <c r="F42" s="4">
-        <v>0</v>
-      </c>
-      <c r="G42" s="4">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="G42" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>71</v>
@@ -3673,15 +3672,15 @@
         <v>216</v>
       </c>
       <c r="F43" s="4">
-        <v>0</v>
-      </c>
-      <c r="G43" s="4">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="G43" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>72</v>
@@ -3696,15 +3695,15 @@
         <v>220</v>
       </c>
       <c r="F44" s="4">
-        <v>0</v>
-      </c>
-      <c r="G44" s="4">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="G44" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>73</v>
@@ -3719,15 +3718,15 @@
         <v>224</v>
       </c>
       <c r="F45" s="4">
-        <v>0</v>
-      </c>
-      <c r="G45" s="4">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="G45" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>74</v>
@@ -3742,15 +3741,15 @@
         <v>228</v>
       </c>
       <c r="F46" s="4">
-        <v>0</v>
-      </c>
-      <c r="G46" s="4">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="G46" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>75</v>
@@ -3765,15 +3764,15 @@
         <v>232</v>
       </c>
       <c r="F47" s="4">
-        <v>0</v>
-      </c>
-      <c r="G47" s="4">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="G47" s="5">
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>76</v>
@@ -3788,15 +3787,15 @@
         <v>236</v>
       </c>
       <c r="F48" s="4">
-        <v>0</v>
-      </c>
-      <c r="G48" s="4">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="G48" s="5">
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>242</v>
@@ -3811,15 +3810,15 @@
         <v>244</v>
       </c>
       <c r="F49" s="4">
-        <v>0</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="G49" s="5">
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>241</v>
@@ -3834,15 +3833,15 @@
         <v>244</v>
       </c>
       <c r="F50" s="4">
-        <v>0</v>
-      </c>
-      <c r="G50" s="4">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="G50" s="5">
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>79</v>
@@ -3857,15 +3856,15 @@
         <v>81</v>
       </c>
       <c r="F51" s="4">
-        <v>0</v>
-      </c>
-      <c r="G51" s="4">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="G51" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>83</v>
@@ -3880,15 +3879,15 @@
         <v>85</v>
       </c>
       <c r="F52" s="4">
-        <v>0</v>
-      </c>
-      <c r="G52" s="4">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="G52" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>87</v>
@@ -3903,15 +3902,15 @@
         <v>89</v>
       </c>
       <c r="F53" s="4">
-        <v>0</v>
-      </c>
-      <c r="G53" s="4">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="G53" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>91</v>
@@ -3926,15 +3925,15 @@
         <v>93</v>
       </c>
       <c r="F54" s="4">
-        <v>0</v>
-      </c>
-      <c r="G54" s="4">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="G54" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>95</v>
@@ -3949,15 +3948,15 @@
         <v>97</v>
       </c>
       <c r="F55" s="4">
-        <v>0</v>
-      </c>
-      <c r="G55" s="4">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="G55" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>99</v>
@@ -3972,15 +3971,15 @@
         <v>101</v>
       </c>
       <c r="F56" s="4">
-        <v>0</v>
-      </c>
-      <c r="G56" s="4">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="G56" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>103</v>
@@ -3995,15 +3994,15 @@
         <v>105</v>
       </c>
       <c r="F57" s="4">
-        <v>0</v>
-      </c>
-      <c r="G57" s="4">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="G57" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>107</v>
@@ -4018,15 +4017,15 @@
         <v>109</v>
       </c>
       <c r="F58" s="4">
-        <v>0</v>
-      </c>
-      <c r="G58" s="4">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="G58" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>111</v>
@@ -4041,15 +4040,15 @@
         <v>113</v>
       </c>
       <c r="F59" s="4">
-        <v>0</v>
-      </c>
-      <c r="G59" s="4">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="G59" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>115</v>
@@ -4064,15 +4063,15 @@
         <v>117</v>
       </c>
       <c r="F60" s="4">
-        <v>0</v>
-      </c>
-      <c r="G60" s="4">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="G60" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>119</v>
@@ -4087,15 +4086,15 @@
         <v>121</v>
       </c>
       <c r="F61" s="4">
-        <v>0</v>
-      </c>
-      <c r="G61" s="4">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="G61" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>123</v>
@@ -4110,15 +4109,15 @@
         <v>125</v>
       </c>
       <c r="F62" s="4">
-        <v>0</v>
-      </c>
-      <c r="G62" s="4">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="G62" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>265</v>
@@ -4133,15 +4132,15 @@
         <v>128</v>
       </c>
       <c r="F63" s="4">
-        <v>0</v>
-      </c>
-      <c r="G63" s="4">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="G63" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>266</v>
@@ -4156,15 +4155,15 @@
         <v>77</v>
       </c>
       <c r="F64" s="4">
-        <v>0</v>
-      </c>
-      <c r="G64" s="4">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="G64" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>130</v>
@@ -4179,15 +4178,15 @@
         <v>132</v>
       </c>
       <c r="F65" s="4">
-        <v>0</v>
-      </c>
-      <c r="G65" s="4">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="G65" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>133</v>
@@ -4202,15 +4201,15 @@
         <v>135</v>
       </c>
       <c r="F66" s="4">
-        <v>0</v>
-      </c>
-      <c r="G66" s="4">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="G66" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>136</v>
@@ -4225,15 +4224,15 @@
         <v>138</v>
       </c>
       <c r="F67" s="4">
-        <v>0</v>
-      </c>
-      <c r="G67" s="4">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="G67" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>140</v>
@@ -4248,15 +4247,15 @@
         <v>142</v>
       </c>
       <c r="F68" s="4">
-        <v>0</v>
-      </c>
-      <c r="G68" s="4">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="G68" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>143</v>
@@ -4271,15 +4270,15 @@
         <v>145</v>
       </c>
       <c r="F69" s="4">
-        <v>0</v>
-      </c>
-      <c r="G69" s="4">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="G69" s="7">
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>267</v>
@@ -4294,15 +4293,15 @@
         <v>147</v>
       </c>
       <c r="F70" s="4">
-        <v>0</v>
-      </c>
-      <c r="G70" s="4">
-        <v>0</v>
+        <v>69</v>
+      </c>
+      <c r="G70" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>148</v>
@@ -4317,15 +4316,15 @@
         <v>150</v>
       </c>
       <c r="F71" s="4">
-        <v>0</v>
-      </c>
-      <c r="G71" s="4">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="G71" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>151</v>
@@ -4340,15 +4339,15 @@
         <v>153</v>
       </c>
       <c r="F72" s="4">
-        <v>0</v>
-      </c>
-      <c r="G72" s="4">
-        <v>0</v>
+        <v>71</v>
+      </c>
+      <c r="G72" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>155</v>
@@ -4363,15 +4362,15 @@
         <v>157</v>
       </c>
       <c r="F73" s="4">
-        <v>0</v>
-      </c>
-      <c r="G73" s="4">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="G73" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>264</v>
@@ -4386,15 +4385,15 @@
         <v>160</v>
       </c>
       <c r="F74" s="4">
-        <v>0</v>
-      </c>
-      <c r="G74" s="4">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="G74" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>263</v>
@@ -4409,15 +4408,15 @@
         <v>163</v>
       </c>
       <c r="F75" s="4">
-        <v>0</v>
-      </c>
-      <c r="G75" s="4">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="G75" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>165</v>
@@ -4432,15 +4431,15 @@
         <v>167</v>
       </c>
       <c r="F76" s="4">
-        <v>0</v>
-      </c>
-      <c r="G76" s="4">
-        <v>0</v>
+        <v>75</v>
+      </c>
+      <c r="G76" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>169</v>
@@ -4455,15 +4454,15 @@
         <v>171</v>
       </c>
       <c r="F77" s="4">
-        <v>0</v>
-      </c>
-      <c r="G77" s="4">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="G77" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>173</v>
@@ -4478,15 +4477,15 @@
         <v>175</v>
       </c>
       <c r="F78" s="4">
-        <v>0</v>
-      </c>
-      <c r="G78" s="4">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="G78" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>177</v>
@@ -4501,15 +4500,15 @@
         <v>179</v>
       </c>
       <c r="F79" s="4">
-        <v>0</v>
-      </c>
-      <c r="G79" s="4">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="G79" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>181</v>
@@ -4524,15 +4523,15 @@
         <v>183</v>
       </c>
       <c r="F80" s="4">
-        <v>0</v>
-      </c>
-      <c r="G80" s="4">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="G80" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>184</v>
@@ -4547,15 +4546,15 @@
         <v>186</v>
       </c>
       <c r="F81" s="4">
-        <v>0</v>
-      </c>
-      <c r="G81" s="4">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="G81" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>188</v>
@@ -4570,15 +4569,15 @@
         <v>190</v>
       </c>
       <c r="F82" s="4">
-        <v>0</v>
-      </c>
-      <c r="G82" s="4">
-        <v>0</v>
+        <v>81</v>
+      </c>
+      <c r="G82" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>192</v>
@@ -4593,15 +4592,15 @@
         <v>194</v>
       </c>
       <c r="F83" s="4">
-        <v>0</v>
-      </c>
-      <c r="G83" s="4">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="G83" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>196</v>
@@ -4616,15 +4615,15 @@
         <v>198</v>
       </c>
       <c r="F84" s="4">
-        <v>0</v>
-      </c>
-      <c r="G84" s="4">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="G84" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>200</v>
@@ -4639,15 +4638,15 @@
         <v>202</v>
       </c>
       <c r="F85" s="4">
-        <v>0</v>
-      </c>
-      <c r="G85" s="4">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="G85" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>204</v>
@@ -4662,15 +4661,15 @@
         <v>206</v>
       </c>
       <c r="F86" s="4">
-        <v>0</v>
-      </c>
-      <c r="G86" s="4">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="G86" s="7">
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>262</v>
@@ -4685,15 +4684,15 @@
         <v>77</v>
       </c>
       <c r="F87" s="4">
-        <v>0</v>
-      </c>
-      <c r="G87" s="4">
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="G87" s="7">
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>210</v>
@@ -4708,15 +4707,15 @@
         <v>77</v>
       </c>
       <c r="F88" s="4">
-        <v>0</v>
-      </c>
-      <c r="G88" s="4">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="G88" s="7">
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>213</v>
@@ -4731,15 +4730,15 @@
         <v>215</v>
       </c>
       <c r="F89" s="4">
-        <v>0</v>
-      </c>
-      <c r="G89" s="4">
-        <v>0</v>
+        <v>88</v>
+      </c>
+      <c r="G89" s="7">
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>217</v>
@@ -4754,15 +4753,15 @@
         <v>219</v>
       </c>
       <c r="F90" s="4">
-        <v>0</v>
-      </c>
-      <c r="G90" s="4">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="G90" s="7">
+        <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>221</v>
@@ -4777,15 +4776,15 @@
         <v>223</v>
       </c>
       <c r="F91" s="4">
-        <v>0</v>
-      </c>
-      <c r="G91" s="4">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="G91" s="7">
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>225</v>
@@ -4800,15 +4799,15 @@
         <v>227</v>
       </c>
       <c r="F92" s="4">
-        <v>0</v>
-      </c>
-      <c r="G92" s="4">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="G92" s="7">
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>229</v>
@@ -4823,15 +4822,15 @@
         <v>231</v>
       </c>
       <c r="F93" s="4">
-        <v>0</v>
-      </c>
-      <c r="G93" s="4">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="G93" s="7">
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>233</v>
@@ -4846,15 +4845,15 @@
         <v>235</v>
       </c>
       <c r="F94" s="4">
-        <v>0</v>
-      </c>
-      <c r="G94" s="4">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="G94" s="7">
+        <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>237</v>
@@ -4869,10 +4868,10 @@
         <v>239</v>
       </c>
       <c r="F95" s="4">
-        <v>0</v>
-      </c>
-      <c r="G95" s="4">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="G95" s="7">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>